<commit_message>
update 20230505 by xhx ROG
</commit_message>
<xml_diff>
--- a/rules/rules_20230224.xlsx
+++ b/rules/rules_20230224.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D8E251-4461-4BA0-8AD4-DF30D5EF186E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5B0814-927B-46E9-9BEE-975AAF6EC31E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
   <si>
     <t>protocol</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -96,6 +96,26 @@
   </si>
   <si>
     <t>passive1</t>
+  </si>
+  <si>
+    <t>ISI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>active2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IRREG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -435,22 +455,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
-    <col min="2" max="5" width="13.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.375" style="2" customWidth="1"/>
+    <col min="2" max="5" width="13.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.75" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +496,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -490,7 +514,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -501,8 +525,11 @@
       <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -516,7 +543,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="E3" s="2">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -527,8 +554,11 @@
       <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -542,7 +572,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="E4" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -553,8 +583,11 @@
       <c r="H4" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -562,13 +595,13 @@
         <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>4.0599999999999996</v>
+        <v>16.239999999999998</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -579,8 +612,11 @@
       <c r="H5" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -588,10 +624,10 @@
         <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2">
-        <v>8.1199999999999992</v>
+        <v>16.239999999999998</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -605,8 +641,11 @@
       <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -614,13 +653,13 @@
         <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
-        <v>16.239999999999998</v>
+        <v>32.479999999999997</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -631,8 +670,11 @@
       <c r="H7" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -657,8 +699,11 @@
       <c r="H8" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -683,8 +728,11 @@
       <c r="H9" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -692,13 +740,13 @@
         <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2">
-        <v>8.1199999999999992</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="E10" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -709,8 +757,11 @@
       <c r="H10" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -721,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="2">
-        <v>16.239999999999998</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -735,8 +786,11 @@
       <c r="H11" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -744,13 +798,13 @@
         <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2">
-        <v>32.479999999999997</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="E12" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -761,8 +815,11 @@
       <c r="H12" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -770,25 +827,28 @@
         <v>91</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>246.30539999999999</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
       </c>
       <c r="H13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -796,7 +856,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
         <v>4.01</v>
@@ -813,10 +873,13 @@
       <c r="H14" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2">
         <v>93</v>
@@ -825,7 +888,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="2">
-        <v>4.0199999999999996</v>
+        <v>4.01</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -839,19 +902,22 @@
       <c r="H15" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2">
-        <v>4.03</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -865,10 +931,13 @@
       <c r="H16" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2">
         <v>95</v>
@@ -877,7 +946,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="2">
-        <v>4.0599999999999996</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -891,10 +960,13 @@
       <c r="H17" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2">
         <v>96</v>
@@ -903,10 +975,10 @@
         <v>10</v>
       </c>
       <c r="D18" s="2">
-        <v>4</v>
+        <v>4.03</v>
       </c>
       <c r="E18" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -915,24 +987,27 @@
         <v>0</v>
       </c>
       <c r="H18" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2">
         <v>97</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="2">
-        <v>4.0599999999999996</v>
+        <v>4.03</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
@@ -943,8 +1018,11 @@
       <c r="H19" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -952,16 +1030,16 @@
         <v>98</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>246.30539999999999</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
@@ -969,19 +1047,22 @@
       <c r="H20" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="2">
-        <v>4</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
@@ -993,50 +1074,56 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2">
+        <v>100</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="2">
-        <v>152</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2">
-        <v>4.01</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="2">
-        <v>4.0199999999999996</v>
+        <v>4</v>
       </c>
       <c r="E23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="2">
         <v>0</v>
@@ -1045,76 +1132,85 @@
         <v>0</v>
       </c>
       <c r="H23" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="2">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>246.30539999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2">
+        <v>152</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4.01</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="2">
+        <v>153</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="2">
-        <v>4.03</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="2">
-        <v>155</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="2">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2">
-        <v>156</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D26" s="2">
-        <v>4</v>
+        <v>4.01</v>
       </c>
       <c r="E26" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -1123,24 +1219,27 @@
         <v>0</v>
       </c>
       <c r="H26" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="2">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="2">
-        <v>4.0599999999999996</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E27" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
@@ -1151,25 +1250,28 @@
       <c r="H27" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="2">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2">
-        <v>0</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>246.30539999999999</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
         <v>0</v>
@@ -1177,22 +1279,25 @@
       <c r="H28" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="2">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="2">
-        <v>8</v>
+        <v>4.03</v>
       </c>
       <c r="E29" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2">
         <v>0</v>
@@ -1203,45 +1308,51 @@
       <c r="H29" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="2">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D30" s="2">
-        <v>0</v>
+        <v>4.03</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
       </c>
       <c r="H30" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="2">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" s="2">
-        <v>4</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -1250,24 +1361,27 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H31" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="2">
-        <v>4.01</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="E32" s="2">
         <v>0</v>
@@ -1276,131 +1390,146 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H32" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" s="2">
-        <v>4.0199999999999996</v>
+        <v>4</v>
       </c>
       <c r="E33" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="2">
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H33" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B34" s="2">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="2">
-        <v>4.03</v>
+        <v>4</v>
       </c>
       <c r="E34" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="2">
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H34" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I34" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B35" s="2">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D35" s="2">
-        <v>4.0599999999999996</v>
+        <v>8</v>
       </c>
       <c r="E35" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H35" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B36" s="2">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D36" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="G36" s="2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H36" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" s="2">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37" s="2">
-        <v>4.0599999999999996</v>
+        <v>4.01</v>
       </c>
       <c r="E37" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37" s="2">
         <v>0</v>
@@ -1411,22 +1540,25 @@
       <c r="H37" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38" s="2">
-        <v>8</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E38" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="2">
         <v>0</v>
@@ -1436,6 +1568,183 @@
       </c>
       <c r="H38" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="I38" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="2">
+        <v>183</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4.03</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>600</v>
+      </c>
+      <c r="H39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="2">
+        <v>184</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>600</v>
+      </c>
+      <c r="H40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="2">
+        <v>185</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>600</v>
+      </c>
+      <c r="H41" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="2">
+        <v>186</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="2">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>600</v>
+      </c>
+      <c r="H42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="2">
+        <v>187</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="2">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>600</v>
+      </c>
+      <c r="H43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="2">
+        <v>188</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="2">
+        <v>8</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>600</v>
+      </c>
+      <c r="H44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>